<commit_message>
for beta no byebugs
Former-commit-id: 3ee8799cbc46b314bc92c65431582c5eca450281
</commit_message>
<xml_diff>
--- a/db/dummydata/speedtrans/speedtrans__local_charges.xlsx
+++ b/db/dummydata/speedtrans/speedtrans__local_charges.xlsx
@@ -130,10 +130,10 @@
     <t>PER_BILL</t>
   </si>
   <si>
-    <t>Customs Clearance</t>
-  </si>
-  <si>
-    <t>CUST</t>
+    <t>Export Declaration</t>
+  </si>
+  <si>
+    <t>EXP</t>
   </si>
   <si>
     <t>Jeddah</t>

</xml_diff>